<commit_message>
Change List: 1) Export Report Done.
</commit_message>
<xml_diff>
--- a/SimplePlatform/ExportTemplate/Excel/Template.xlsx
+++ b/SimplePlatform/ExportTemplate/Excel/Template.xlsx
@@ -17,7 +17,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -27,6 +31,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -51,15 +62,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="currencyamount" xfId="3"/>
+    <cellStyle name="dateformat" xfId="2"/>
     <cellStyle name="header1" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>

</xml_diff>